<commit_message>
Atualizações ppt,conceitual e logico
</commit_message>
<xml_diff>
--- a/documentacao/Planilhas/Teste_Homologação.xlsx
+++ b/documentacao/Planilhas/Teste_Homologação.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\OneDrive\Área de Trabalho\PI\TechHumi\documentacao\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{DBD25669-B0AB-4980-A57C-C924727D11A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{85639AD4-3C2F-4EE7-8C99-EEC6C98BEE0F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB907EAB-D118-483D-8A8E-F4D49993E41F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
@@ -1312,7 +1312,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1672,6 +1672,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1708,7 +1731,64 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="15" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1718,35 +1798,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1759,31 +1810,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2380,15 +2406,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>258535</xdr:colOff>
+      <xdr:colOff>492125</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>50902</xdr:rowOff>
+      <xdr:rowOff>230275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1827888</xdr:colOff>
+      <xdr:colOff>1716763</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>1156607</xdr:rowOff>
+      <xdr:rowOff>1093107</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2411,8 +2437,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12926785" y="9004402"/>
-          <a:ext cx="1569353" cy="1105705"/>
+          <a:off x="13160375" y="10009275"/>
+          <a:ext cx="1224638" cy="862832"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2468,15 +2494,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>367392</xdr:colOff>
+      <xdr:colOff>603250</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>56891</xdr:rowOff>
+      <xdr:rowOff>62840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1811832</xdr:colOff>
+      <xdr:colOff>1526081</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>1040511</xdr:rowOff>
+      <xdr:rowOff>691260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2499,8 +2525,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13035642" y="10275855"/>
-          <a:ext cx="1444440" cy="983620"/>
+          <a:off x="13271500" y="11318215"/>
+          <a:ext cx="922831" cy="628420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2514,13 +2540,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>215515</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>231322</xdr:rowOff>
+      <xdr:rowOff>78922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1240333</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>929192</xdr:rowOff>
+      <xdr:rowOff>779967</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2543,8 +2569,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18136122" y="10450286"/>
-          <a:ext cx="1024818" cy="697870"/>
+          <a:off x="18160615" y="11356522"/>
+          <a:ext cx="1024818" cy="701045"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2556,15 +2582,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>275652</xdr:colOff>
+      <xdr:colOff>384941</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>68035</xdr:rowOff>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1787068</xdr:colOff>
+      <xdr:colOff>1564817</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>1132920</xdr:rowOff>
+      <xdr:rowOff>990045</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2587,8 +2613,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12943902" y="11375571"/>
-          <a:ext cx="1511416" cy="1064885"/>
+          <a:off x="13053191" y="12366625"/>
+          <a:ext cx="1179876" cy="831295"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2600,15 +2626,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>136073</xdr:colOff>
+      <xdr:colOff>183698</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>225765</xdr:rowOff>
+      <xdr:rowOff>194015</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1075987</xdr:colOff>
+      <xdr:colOff>1123612</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>887992</xdr:rowOff>
+      <xdr:rowOff>856242</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2631,7 +2657,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18056680" y="11533301"/>
+          <a:off x="18106573" y="12401890"/>
           <a:ext cx="939914" cy="662227"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3319,19 +3345,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
     <col min="4" max="5" width="16.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="40.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="16.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" style="2" customWidth="1"/>
     <col min="12" max="12" width="20.5703125" style="2" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" style="2" customWidth="1"/>
@@ -3358,13 +3386,13 @@
     </row>
     <row r="2" spans="1:20" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="47"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="107"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="113"/>
       <c r="G2" s="51"/>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
@@ -3374,11 +3402,11 @@
     </row>
     <row r="3" spans="1:20" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="47"/>
-      <c r="B3" s="108"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="110"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="116"/>
       <c r="G3" s="51"/>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
@@ -3405,10 +3433,10 @@
       <c r="B5" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="111" t="s">
+      <c r="C5" s="117" t="s">
         <v>170</v>
       </c>
-      <c r="D5" s="112"/>
+      <c r="D5" s="118"/>
       <c r="E5" s="26"/>
       <c r="F5" s="27"/>
       <c r="G5" s="26"/>
@@ -3423,10 +3451,10 @@
       <c r="B6" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="111" t="s">
+      <c r="C6" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="D6" s="112"/>
+      <c r="D6" s="118"/>
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
       <c r="G6" s="26"/>
@@ -3441,10 +3469,10 @@
       <c r="B7" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="111" t="s">
+      <c r="C7" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="112"/>
+      <c r="D7" s="118"/>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="26"/>
@@ -3459,10 +3487,10 @@
       <c r="B8" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="111" t="s">
+      <c r="C8" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="112"/>
+      <c r="D8" s="118"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
       <c r="G8" s="26"/>
@@ -3472,25 +3500,26 @@
       <c r="K8" s="26"/>
       <c r="L8" s="22"/>
     </row>
-    <row r="9" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="55" t="s">
+    <row r="9" spans="1:20" s="109" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="106"/>
+      <c r="B9" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="116">
+      <c r="C9" s="122">
         <v>43619</v>
       </c>
-      <c r="D9" s="112"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="D9" s="123"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="106"/>
+      <c r="P9" s="110"/>
+    </row>
+    <row r="10" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -3504,37 +3533,37 @@
       <c r="K10" s="26"/>
       <c r="L10" s="22"/>
     </row>
-    <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="123"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="127"/>
       <c r="J11" s="26"/>
       <c r="K11" s="26"/>
       <c r="L11" s="22"/>
       <c r="O11" s="3"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:20" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="4" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
       <c r="B12" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="136" t="s">
+      <c r="C12" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="137"/>
-      <c r="E12" s="136" t="s">
+      <c r="D12" s="129"/>
+      <c r="E12" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="137"/>
+      <c r="F12" s="129"/>
       <c r="G12" s="65" t="s">
         <v>21</v>
       </c>
@@ -3557,14 +3586,14 @@
       <c r="B13" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="113" t="s">
+      <c r="C13" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="115"/>
-      <c r="E13" s="113" t="s">
+      <c r="D13" s="121"/>
+      <c r="E13" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="115"/>
+      <c r="F13" s="121"/>
       <c r="G13" s="58" t="s">
         <v>87</v>
       </c>
@@ -3587,14 +3616,14 @@
       <c r="B14" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="126" t="s">
+      <c r="C14" s="132" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="127"/>
-      <c r="E14" s="126" t="s">
+      <c r="D14" s="133"/>
+      <c r="E14" s="132" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="127"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="67" t="s">
         <v>88</v>
       </c>
@@ -3617,14 +3646,14 @@
       <c r="B15" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="115"/>
-      <c r="E15" s="113" t="s">
+      <c r="D15" s="121"/>
+      <c r="E15" s="119" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="138"/>
+      <c r="F15" s="124"/>
       <c r="G15" s="58" t="s">
         <v>89</v>
       </c>
@@ -3647,14 +3676,14 @@
       <c r="B16" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="113" t="s">
+      <c r="C16" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="114"/>
-      <c r="E16" s="113" t="s">
+      <c r="D16" s="120"/>
+      <c r="E16" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="114"/>
+      <c r="F16" s="120"/>
       <c r="G16" s="58" t="s">
         <v>96</v>
       </c>
@@ -3677,14 +3706,14 @@
       <c r="B17" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="113" t="s">
+      <c r="C17" s="119" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="114"/>
-      <c r="E17" s="113" t="s">
+      <c r="D17" s="120"/>
+      <c r="E17" s="119" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="114"/>
+      <c r="F17" s="120"/>
       <c r="G17" s="58" t="s">
         <v>95</v>
       </c>
@@ -3707,14 +3736,14 @@
       <c r="B18" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="119" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="114"/>
-      <c r="E18" s="113" t="s">
+      <c r="D18" s="120"/>
+      <c r="E18" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="114"/>
+      <c r="F18" s="120"/>
       <c r="G18" s="58" t="s">
         <v>88</v>
       </c>
@@ -3737,14 +3766,14 @@
       <c r="B19" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="113" t="s">
+      <c r="C19" s="119" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="114"/>
-      <c r="E19" s="117" t="s">
+      <c r="D19" s="120"/>
+      <c r="E19" s="140" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="118"/>
+      <c r="F19" s="141"/>
       <c r="G19" s="58" t="s">
         <v>105</v>
       </c>
@@ -3765,10 +3794,10 @@
     <row r="20" spans="1:21" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
       <c r="B20" s="57"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="138"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="124"/>
       <c r="G20" s="58" t="s">
         <v>104</v>
       </c>
@@ -3802,17 +3831,17 @@
     </row>
     <row r="22" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="49"/>
-      <c r="B22" s="124" t="s">
+      <c r="B22" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="125"/>
-      <c r="F22" s="125"/>
-      <c r="G22" s="125"/>
-      <c r="H22" s="125"/>
-      <c r="I22" s="125"/>
-      <c r="J22" s="125"/>
+      <c r="C22" s="135"/>
+      <c r="D22" s="135"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="135"/>
+      <c r="I22" s="135"/>
+      <c r="J22" s="135"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
     </row>
@@ -3821,18 +3850,18 @@
       <c r="B23" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="119" t="s">
+      <c r="C23" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="120"/>
-      <c r="E23" s="119" t="s">
+      <c r="D23" s="131"/>
+      <c r="E23" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="120"/>
-      <c r="G23" s="119" t="s">
+      <c r="F23" s="131"/>
+      <c r="G23" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="120"/>
+      <c r="H23" s="131"/>
       <c r="I23" s="64" t="s">
         <v>23</v>
       </c>
@@ -3846,23 +3875,23 @@
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
     </row>
-    <row r="24" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
       <c r="B24" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="113" t="s">
+      <c r="C24" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="115"/>
-      <c r="E24" s="113" t="s">
+      <c r="D24" s="121"/>
+      <c r="E24" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="F24" s="115"/>
-      <c r="G24" s="113" t="s">
+      <c r="F24" s="121"/>
+      <c r="G24" s="119" t="s">
         <v>137</v>
       </c>
-      <c r="H24" s="115"/>
+      <c r="H24" s="121"/>
       <c r="I24" s="59" t="s">
         <v>86</v>
       </c>
@@ -3876,23 +3905,23 @@
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
     </row>
-    <row r="25" spans="1:21" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" s="4" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
       <c r="B25" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="113" t="s">
+      <c r="C25" s="119" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="114"/>
-      <c r="E25" s="132" t="s">
+      <c r="D25" s="120"/>
+      <c r="E25" s="136" t="s">
         <v>139</v>
       </c>
-      <c r="F25" s="133"/>
-      <c r="G25" s="134" t="s">
+      <c r="F25" s="137"/>
+      <c r="G25" s="138" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="135"/>
+      <c r="H25" s="139"/>
       <c r="I25" s="60" t="s">
         <v>86</v>
       </c>
@@ -3906,23 +3935,23 @@
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
     </row>
-    <row r="26" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="48"/>
       <c r="B26" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="113" t="s">
+      <c r="C26" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="114"/>
-      <c r="E26" s="132" t="s">
+      <c r="D26" s="120"/>
+      <c r="E26" s="136" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="133"/>
-      <c r="G26" s="134" t="s">
+      <c r="F26" s="137"/>
+      <c r="G26" s="138" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="135"/>
+      <c r="H26" s="139"/>
       <c r="I26" s="60" t="s">
         <v>86</v>
       </c>
@@ -3936,23 +3965,23 @@
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" s="4" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="48"/>
       <c r="B27" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="113" t="s">
+      <c r="C27" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="D27" s="114"/>
-      <c r="E27" s="132" t="s">
+      <c r="D27" s="120"/>
+      <c r="E27" s="136" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="133"/>
-      <c r="G27" s="134" t="s">
+      <c r="F27" s="137"/>
+      <c r="G27" s="138" t="s">
         <v>122</v>
       </c>
-      <c r="H27" s="135"/>
+      <c r="H27" s="139"/>
       <c r="I27" s="70" t="s">
         <v>86</v>
       </c>
@@ -3966,23 +3995,23 @@
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
     </row>
-    <row r="28" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="48"/>
       <c r="B28" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="113" t="s">
+      <c r="C28" s="119" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="114"/>
-      <c r="E28" s="132" t="s">
+      <c r="D28" s="120"/>
+      <c r="E28" s="136" t="s">
         <v>111</v>
       </c>
-      <c r="F28" s="133"/>
-      <c r="G28" s="134" t="s">
+      <c r="F28" s="137"/>
+      <c r="G28" s="138" t="s">
         <v>112</v>
       </c>
-      <c r="H28" s="135"/>
+      <c r="H28" s="139"/>
       <c r="I28" s="70" t="s">
         <v>86</v>
       </c>
@@ -3996,23 +4025,23 @@
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
     </row>
-    <row r="29" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="48"/>
       <c r="B29" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="113" t="s">
+      <c r="C29" s="119" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="114"/>
-      <c r="E29" s="132" t="s">
+      <c r="D29" s="120"/>
+      <c r="E29" s="136" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="133"/>
-      <c r="G29" s="134" t="s">
+      <c r="F29" s="137"/>
+      <c r="G29" s="138" t="s">
         <v>127</v>
       </c>
-      <c r="H29" s="135"/>
+      <c r="H29" s="139"/>
       <c r="I29" s="70" t="s">
         <v>128</v>
       </c>
@@ -4026,23 +4055,23 @@
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
     </row>
-    <row r="30" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="4" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="48"/>
       <c r="B30" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="C30" s="113" t="s">
+      <c r="C30" s="119" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="114"/>
-      <c r="E30" s="132" t="s">
+      <c r="D30" s="120"/>
+      <c r="E30" s="136" t="s">
         <v>114</v>
       </c>
-      <c r="F30" s="133"/>
-      <c r="G30" s="134" t="s">
+      <c r="F30" s="137"/>
+      <c r="G30" s="138" t="s">
         <v>115</v>
       </c>
-      <c r="H30" s="135"/>
+      <c r="H30" s="139"/>
       <c r="I30" s="58" t="s">
         <v>86</v>
       </c>
@@ -4056,7 +4085,7 @@
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
     </row>
-    <row r="31" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" s="4" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="48"/>
       <c r="B31" s="57" t="s">
         <v>129</v>
@@ -4065,14 +4094,14 @@
         <v>131</v>
       </c>
       <c r="D31" s="85"/>
-      <c r="E31" s="139" t="s">
+      <c r="E31" s="146" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="140"/>
-      <c r="G31" s="141" t="s">
+      <c r="F31" s="147"/>
+      <c r="G31" s="148" t="s">
         <v>133</v>
       </c>
-      <c r="H31" s="142"/>
+      <c r="H31" s="149"/>
       <c r="I31" s="58" t="s">
         <v>86</v>
       </c>
@@ -4089,12 +4118,12 @@
     <row r="32" spans="1:21" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="48"/>
       <c r="B32" s="83"/>
-      <c r="C32" s="143"/>
-      <c r="D32" s="143"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="145"/>
-      <c r="H32" s="145"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
+      <c r="G32" s="152"/>
+      <c r="H32" s="152"/>
       <c r="I32" s="84"/>
       <c r="J32" s="80"/>
       <c r="K32" s="25"/>
@@ -4107,12 +4136,12 @@
     <row r="33" spans="1:21" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="48"/>
       <c r="B33" s="82"/>
-      <c r="C33" s="129"/>
-      <c r="D33" s="129"/>
-      <c r="E33" s="146"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="147"/>
-      <c r="H33" s="147"/>
+      <c r="C33" s="143"/>
+      <c r="D33" s="143"/>
+      <c r="E33" s="153"/>
+      <c r="F33" s="153"/>
+      <c r="G33" s="154"/>
+      <c r="H33" s="154"/>
       <c r="I33" s="80"/>
       <c r="J33" s="80"/>
       <c r="K33" s="25"/>
@@ -4125,12 +4154,12 @@
     <row r="34" spans="1:21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="48"/>
       <c r="B34" s="82"/>
-      <c r="C34" s="129"/>
-      <c r="D34" s="129"/>
-      <c r="E34" s="148"/>
-      <c r="F34" s="148"/>
-      <c r="G34" s="147"/>
-      <c r="H34" s="147"/>
+      <c r="C34" s="143"/>
+      <c r="D34" s="143"/>
+      <c r="E34" s="155"/>
+      <c r="F34" s="155"/>
+      <c r="G34" s="154"/>
+      <c r="H34" s="154"/>
       <c r="I34" s="80"/>
       <c r="J34" s="80"/>
       <c r="K34" s="25"/>
@@ -4143,12 +4172,12 @@
     <row r="35" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="48"/>
       <c r="B35" s="82"/>
-      <c r="C35" s="129"/>
-      <c r="D35" s="130"/>
-      <c r="E35" s="129"/>
-      <c r="F35" s="131"/>
-      <c r="G35" s="128"/>
-      <c r="H35" s="128"/>
+      <c r="C35" s="143"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="143"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="142"/>
+      <c r="H35" s="142"/>
       <c r="I35" s="80"/>
       <c r="J35" s="80"/>
       <c r="K35" s="25"/>
@@ -4299,17 +4328,10 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
@@ -4322,26 +4344,28 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B22:J22"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="C5:D5"/>
@@ -4353,6 +4377,11 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J24:J35" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -4375,8 +4404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView topLeftCell="B30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4483,10 +4512,10 @@
       <c r="A15" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="152" t="s">
+      <c r="B15" s="159" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="152"/>
+      <c r="C15" s="159"/>
       <c r="D15" s="39"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -4542,7 +4571,7 @@
       <c r="S24" s="42"/>
       <c r="T24" s="42"/>
     </row>
-    <row r="25" spans="1:20" s="41" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="41" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="40" t="s">
         <v>142</v>
       </c>
@@ -4573,7 +4602,7 @@
       <c r="S25" s="42"/>
       <c r="T25" s="42"/>
     </row>
-    <row r="26" spans="1:20" s="41" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="41" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="40" t="s">
         <v>143</v>
       </c>
@@ -4635,7 +4664,7 @@
       <c r="S27" s="42"/>
       <c r="T27" s="42"/>
     </row>
-    <row r="28" spans="1:20" s="41" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" s="41" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="40" t="s">
         <v>117</v>
       </c>
@@ -4666,7 +4695,7 @@
       <c r="S28" s="42"/>
       <c r="T28" s="42"/>
     </row>
-    <row r="29" spans="1:20" s="41" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" s="41" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="40" t="s">
         <v>118</v>
       </c>
@@ -4697,7 +4726,7 @@
       <c r="S29" s="42"/>
       <c r="T29" s="42"/>
     </row>
-    <row r="30" spans="1:20" s="41" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" s="41" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="40" t="s">
         <v>165</v>
       </c>
@@ -4911,12 +4940,12 @@
     </row>
     <row r="40" spans="1:20" s="41" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="82"/>
-      <c r="B40" s="149"/>
-      <c r="C40" s="153"/>
-      <c r="D40" s="149"/>
-      <c r="E40" s="153"/>
-      <c r="F40" s="149"/>
-      <c r="G40" s="153"/>
+      <c r="B40" s="156"/>
+      <c r="C40" s="160"/>
+      <c r="D40" s="156"/>
+      <c r="E40" s="160"/>
+      <c r="F40" s="156"/>
+      <c r="G40" s="160"/>
       <c r="H40" s="78"/>
       <c r="I40" s="79"/>
       <c r="J40" s="77"/>
@@ -4927,12 +4956,12 @@
     </row>
     <row r="41" spans="1:20" s="41" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="82"/>
-      <c r="B41" s="149"/>
-      <c r="C41" s="149"/>
-      <c r="D41" s="150"/>
-      <c r="E41" s="150"/>
-      <c r="F41" s="151"/>
-      <c r="G41" s="151"/>
+      <c r="B41" s="156"/>
+      <c r="C41" s="156"/>
+      <c r="D41" s="157"/>
+      <c r="E41" s="157"/>
+      <c r="F41" s="158"/>
+      <c r="G41" s="158"/>
       <c r="H41" s="79"/>
       <c r="I41" s="79"/>
       <c r="J41" s="77"/>
@@ -4943,12 +4972,12 @@
     </row>
     <row r="42" spans="1:20" s="41" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="82"/>
-      <c r="B42" s="149"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="150"/>
-      <c r="E42" s="150"/>
-      <c r="F42" s="151"/>
-      <c r="G42" s="151"/>
+      <c r="B42" s="156"/>
+      <c r="C42" s="156"/>
+      <c r="D42" s="157"/>
+      <c r="E42" s="157"/>
+      <c r="F42" s="158"/>
+      <c r="G42" s="158"/>
       <c r="H42" s="79"/>
       <c r="I42" s="79"/>
       <c r="J42" s="77"/>
@@ -4959,12 +4988,12 @@
     </row>
     <row r="43" spans="1:20" s="41" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="82"/>
-      <c r="B43" s="149"/>
-      <c r="C43" s="149"/>
-      <c r="D43" s="150"/>
-      <c r="E43" s="150"/>
-      <c r="F43" s="151"/>
-      <c r="G43" s="151"/>
+      <c r="B43" s="156"/>
+      <c r="C43" s="156"/>
+      <c r="D43" s="157"/>
+      <c r="E43" s="157"/>
+      <c r="F43" s="158"/>
+      <c r="G43" s="158"/>
       <c r="H43" s="79"/>
       <c r="I43" s="79"/>
       <c r="J43" s="77"/>
@@ -4975,12 +5004,12 @@
     </row>
     <row r="44" spans="1:20" s="41" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="82"/>
-      <c r="B44" s="129"/>
-      <c r="C44" s="129"/>
-      <c r="D44" s="146"/>
-      <c r="E44" s="146"/>
-      <c r="F44" s="147"/>
-      <c r="G44" s="147"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="143"/>
+      <c r="D44" s="153"/>
+      <c r="E44" s="153"/>
+      <c r="F44" s="154"/>
+      <c r="G44" s="154"/>
       <c r="H44" s="80"/>
       <c r="I44" s="80"/>
       <c r="Q44" s="42"/>
@@ -4990,12 +5019,12 @@
     </row>
     <row r="45" spans="1:20" s="41" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A45" s="82"/>
-      <c r="B45" s="129"/>
-      <c r="C45" s="129"/>
-      <c r="D45" s="146"/>
-      <c r="E45" s="146"/>
-      <c r="F45" s="147"/>
-      <c r="G45" s="147"/>
+      <c r="B45" s="143"/>
+      <c r="C45" s="143"/>
+      <c r="D45" s="153"/>
+      <c r="E45" s="153"/>
+      <c r="F45" s="154"/>
+      <c r="G45" s="154"/>
       <c r="H45" s="80"/>
       <c r="I45" s="80"/>
       <c r="J45" s="74"/>
@@ -5094,8 +5123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5112,20 +5141,20 @@
     <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="104"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="156"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="163"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="159"/>
+      <c r="B3" s="164"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="166"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
@@ -5392,28 +5421,28 @@
       <c r="F21" s="15"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="161" t="s">
+      <c r="B22" s="168" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="162" t="s">
+      <c r="D22" s="169" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="162"/>
-      <c r="F22" s="162"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="161"/>
+      <c r="B23" s="168"/>
       <c r="C23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="162" t="s">
+      <c r="D23" s="169" t="s">
         <v>187</v>
       </c>
-      <c r="E23" s="162"/>
-      <c r="F23" s="162"/>
+      <c r="E23" s="169"/>
+      <c r="F23" s="169"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="101"/>
@@ -5445,9 +5474,9 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="14"/>
-      <c r="C29" s="160"/>
-      <c r="D29" s="160"/>
-      <c r="E29" s="160"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
       <c r="F29" s="15"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>